<commit_message>
New chapter in the LCA notebook: Life Cycle Impact Assessment, all results checked. Still to do: graphs and energy mix.
</commit_message>
<xml_diff>
--- a/files/LCI_CW_EoL.xlsx
+++ b/files/LCI_CW_EoL.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\souvi\Documents\These\80_Calculations\05_LCA_Repo\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\souvi\Documents\These\80_Calculations\05_LCA\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0237155-697F-4C7B-A5BF-DDFC3411AB49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9212E63-FE23-434D-8D36-4B68536763D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="688" firstSheet="7" activeTab="10" xr2:uid="{C53D2317-A0AE-4D89-AE6C-E52C75B15043}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="688" firstSheet="1" activeTab="1" xr2:uid="{C53D2317-A0AE-4D89-AE6C-E52C75B15043}"/>
   </bookViews>
   <sheets>
     <sheet name="Hypothesis" sheetId="1" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2434" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2434" uniqueCount="280">
   <si>
     <t>skip</t>
   </si>
@@ -335,9 +335,6 @@
     <t>Database parameters</t>
   </si>
   <si>
-    <t>exldb_cw_EoL</t>
-  </si>
-  <si>
     <t>kg/m³</t>
   </si>
   <si>
@@ -614,21 +611,6 @@
     <t>param_m_dsf_alu</t>
   </si>
   <si>
-    <t>param_d3 * param_m_sg_g</t>
-  </si>
-  <si>
-    <t>param_d3 * param_m_dg_g</t>
-  </si>
-  <si>
-    <t>param_d3 * param_m_tg_g</t>
-  </si>
-  <si>
-    <t>param_d2 * (param_m_dg_g + param_m_dg_alu)</t>
-  </si>
-  <si>
-    <t>param_d2 * (param_m_tg_g + param_m_tg_alu)</t>
-  </si>
-  <si>
     <t>market for used curtain wall, aluminium frame, high performance, for triple glazing</t>
   </si>
   <si>
@@ -650,9 +632,6 @@
     <t>-param_m_ccf_epdm</t>
   </si>
   <si>
-    <t>param_d2 * (param_m_ccf_g + param_m_ccf_alu)</t>
-  </si>
-  <si>
     <t>market for used curtain wall, double skin facade system</t>
   </si>
   <si>
@@ -665,9 +644,6 @@
     <t>-param_m_dsf_alu</t>
   </si>
   <si>
-    <t>param_d2 * (param_m_sg_g + param_m_sg_alu)</t>
-  </si>
-  <si>
     <t>market for used curtain wall, aluminium frame, low performance, for single glazing</t>
   </si>
   <si>
@@ -689,18 +665,12 @@
     <t>treatment for used curtain wall, aluminium frame, vacuum double glazing</t>
   </si>
   <si>
-    <t>param_d2 * (param_m_vacuum_g + param_m_dg_alu)</t>
-  </si>
-  <si>
     <t>eol_vacuum</t>
   </si>
   <si>
     <t>treatment for used curtain wall, closed cavity facade system</t>
   </si>
   <si>
-    <t>param_d3 * param_m_vacuum_g</t>
-  </si>
-  <si>
     <t>-param_m_vacuum_g</t>
   </si>
   <si>
@@ -788,12 +758,6 @@
     <t>total mass of electronic/chromic devices for 1m² of smart double glazing</t>
   </si>
   <si>
-    <t>param_d2 * (param_m_smart_g + param_m_dg_alu + param_m_smart_elec)</t>
-  </si>
-  <si>
-    <t>-param_m_dg_epdm</t>
-  </si>
-  <si>
     <t>treatment for used smart double glazing</t>
   </si>
   <si>
@@ -806,9 +770,6 @@
     <t>market_eol_smart</t>
   </si>
   <si>
-    <t>param_d3 * (param_m_smart_g + param_m_smart_elec)</t>
-  </si>
-  <si>
     <t>market for waste electric and electronic equipment</t>
   </si>
   <si>
@@ -903,6 +864,42 @@
   </si>
   <si>
     <t>RoW</t>
+  </si>
+  <si>
+    <t>exldb_cw_eol</t>
+  </si>
+  <si>
+    <t>param_d2 * (param_m_ccf_g + param_m_ccf_alu) / 1000</t>
+  </si>
+  <si>
+    <t>param_d2 * (param_m_smart_g + param_m_dg_alu + param_m_smart_elec) / 1000</t>
+  </si>
+  <si>
+    <t>param_d2 * (param_m_vacuum_g + param_m_dg_alu) / 1000</t>
+  </si>
+  <si>
+    <t>param_d2 * (param_m_tg_g + param_m_tg_alu) / 1000</t>
+  </si>
+  <si>
+    <t>param_d2 * (param_m_dg_g + param_m_dg_alu) / 1000</t>
+  </si>
+  <si>
+    <t>param_d2 * (param_m_sg_g + param_m_sg_alu) / 1000</t>
+  </si>
+  <si>
+    <t>param_d3 * (param_m_smart_g + param_m_smart_elec) / 1000</t>
+  </si>
+  <si>
+    <t>param_d3 * param_m_vacuum_g / 1000</t>
+  </si>
+  <si>
+    <t>param_d3 * param_m_tg_g / 1000</t>
+  </si>
+  <si>
+    <t>param_d3 * param_m_dg_g / 1000</t>
+  </si>
+  <si>
+    <t>param_d3 * param_m_sg_g / 1000</t>
   </si>
 </sst>
 </file>
@@ -1781,35 +1778,35 @@
     </row>
     <row r="36" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D36">
         <v>1500</v>
       </c>
       <c r="E36" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="37" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C37" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D37">
         <v>2700</v>
       </c>
       <c r="E37" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="38" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C38" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D38">
         <v>1500</v>
       </c>
       <c r="E38" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="40" spans="3:8" x14ac:dyDescent="0.25">
@@ -1914,7 +1911,7 @@
         <v>13</v>
       </c>
       <c r="F48" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="49" spans="3:8" x14ac:dyDescent="0.25">
@@ -1929,7 +1926,7 @@
         <v>82</v>
       </c>
       <c r="F49" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="50" spans="3:8" x14ac:dyDescent="0.25">
@@ -1946,7 +1943,7 @@
     </row>
     <row r="51" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C51" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D51" s="11">
         <f>100/1000000*D38</f>
@@ -1956,7 +1953,7 @@
         <v>13</v>
       </c>
       <c r="F51" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="53" spans="3:8" x14ac:dyDescent="0.25">
@@ -1995,7 +1992,7 @@
         <v>13</v>
       </c>
       <c r="F55" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="56" spans="3:8" x14ac:dyDescent="0.25">
@@ -2010,7 +2007,7 @@
         <v>13</v>
       </c>
       <c r="F56" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="58" spans="3:8" x14ac:dyDescent="0.25">
@@ -2052,7 +2049,7 @@
         <v>13</v>
       </c>
       <c r="F61" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="62" spans="3:8" x14ac:dyDescent="0.25">
@@ -2067,7 +2064,7 @@
         <v>82</v>
       </c>
       <c r="F62" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="63" spans="3:8" x14ac:dyDescent="0.25">
@@ -2084,7 +2081,7 @@
     </row>
     <row r="64" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C64" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D64" s="11">
         <f>100/1000000*D38</f>
@@ -2094,7 +2091,7 @@
         <v>13</v>
       </c>
       <c r="F64" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="66" spans="3:8" x14ac:dyDescent="0.25">
@@ -2133,7 +2130,7 @@
         <v>13</v>
       </c>
       <c r="F68" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="69" spans="3:8" x14ac:dyDescent="0.25">
@@ -2148,7 +2145,7 @@
         <v>13</v>
       </c>
       <c r="F69" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="72" spans="3:8" x14ac:dyDescent="0.25">
@@ -2187,7 +2184,7 @@
         <v>13</v>
       </c>
       <c r="F74" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="75" spans="3:8" x14ac:dyDescent="0.25">
@@ -2202,12 +2199,12 @@
         <v>13</v>
       </c>
       <c r="F75" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="78" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C78" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D78" s="6"/>
       <c r="E78" s="22"/>
@@ -2241,7 +2238,7 @@
         <v>13</v>
       </c>
       <c r="F80" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="81" spans="3:6" x14ac:dyDescent="0.25">
@@ -2256,7 +2253,7 @@
         <v>13</v>
       </c>
       <c r="F81" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -2269,7 +2266,7 @@
   <dimension ref="A1:P19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:XFD12"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2302,7 +2299,7 @@
         <v>39</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="15"/>
@@ -2320,7 +2317,7 @@
         <v>42</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>247</v>
+        <v>235</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="15"/>
@@ -2422,7 +2419,7 @@
     </row>
     <row r="12" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="26" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
       <c r="B12" s="27">
         <v>-1</v>
@@ -2432,7 +2429,7 @@
       </c>
       <c r="D12" s="20"/>
       <c r="E12" s="20" t="s">
-        <v>91</v>
+        <v>268</v>
       </c>
       <c r="F12" s="20" t="s">
         <v>61</v>
@@ -2462,7 +2459,7 @@
         <v>61</v>
       </c>
       <c r="O12" s="20" t="s">
-        <v>264</v>
+        <v>251</v>
       </c>
       <c r="P12" s="26"/>
     </row>
@@ -2477,7 +2474,7 @@
         <v>84</v>
       </c>
       <c r="D13" s="31" t="s">
-        <v>248</v>
+        <v>275</v>
       </c>
       <c r="E13" s="31" t="s">
         <v>60</v>
@@ -2516,7 +2513,7 @@
     </row>
     <row r="14" spans="1:16" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="33" t="s">
-        <v>244</v>
+        <v>232</v>
       </c>
       <c r="B14" s="34">
         <v>-1</v>
@@ -2526,7 +2523,7 @@
       </c>
       <c r="D14" s="31"/>
       <c r="E14" s="31" t="s">
-        <v>91</v>
+        <v>268</v>
       </c>
       <c r="F14" s="31" t="s">
         <v>61</v>
@@ -2556,7 +2553,7 @@
         <v>61</v>
       </c>
       <c r="O14" s="31" t="s">
-        <v>265</v>
+        <v>252</v>
       </c>
       <c r="P14" s="33"/>
     </row>
@@ -2660,8 +2657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EE79EBA-5497-4484-9655-40B62D1F5661}">
   <dimension ref="A1:P17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="O18" sqref="O18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2692,7 +2689,7 @@
         <v>39</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>244</v>
+        <v>232</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="15"/>
@@ -2710,7 +2707,7 @@
         <v>42</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>245</v>
+        <v>233</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="15"/>
@@ -2812,7 +2809,7 @@
     </row>
     <row r="12" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="26" t="s">
-        <v>244</v>
+        <v>232</v>
       </c>
       <c r="B12" s="27">
         <v>-1</v>
@@ -2822,7 +2819,7 @@
       </c>
       <c r="D12" s="20"/>
       <c r="E12" s="20" t="s">
-        <v>91</v>
+        <v>268</v>
       </c>
       <c r="F12" s="20" t="s">
         <v>61</v>
@@ -2852,13 +2849,13 @@
         <v>61</v>
       </c>
       <c r="O12" s="20" t="s">
-        <v>265</v>
+        <v>252</v>
       </c>
       <c r="P12" s="26"/>
     </row>
     <row r="13" spans="1:16" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="33" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="B13" s="40">
         <v>0</v>
@@ -2867,7 +2864,7 @@
         <v>48</v>
       </c>
       <c r="D13" s="42" t="s">
-        <v>246</v>
+        <v>234</v>
       </c>
       <c r="E13" s="31" t="s">
         <v>60</v>
@@ -2876,7 +2873,7 @@
         <v>61</v>
       </c>
       <c r="G13" s="31" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H13" s="31" t="s">
         <v>62</v>
@@ -2900,13 +2897,13 @@
         <v>61</v>
       </c>
       <c r="O13" s="31" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="P13" s="33"/>
     </row>
     <row r="14" spans="1:16" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="33" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B14" s="39">
         <f>-0.35</f>
@@ -2923,7 +2920,7 @@
         <v>61</v>
       </c>
       <c r="G14" s="31" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H14" s="31" t="s">
         <v>62</v>
@@ -2947,13 +2944,13 @@
         <v>61</v>
       </c>
       <c r="O14" s="31" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="P14" s="33"/>
     </row>
     <row r="15" spans="1:16" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="33" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B15" s="39">
         <f>-0.4</f>
@@ -2970,7 +2967,7 @@
         <v>61</v>
       </c>
       <c r="G15" s="31" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H15" s="31" t="s">
         <v>62</v>
@@ -2994,13 +2991,13 @@
         <v>61</v>
       </c>
       <c r="O15" s="31" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="P15" s="33"/>
     </row>
     <row r="16" spans="1:16" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="33" t="s">
-        <v>249</v>
+        <v>236</v>
       </c>
       <c r="B16" s="39">
         <f>-0.12</f>
@@ -3017,7 +3014,7 @@
         <v>61</v>
       </c>
       <c r="G16" s="31" t="s">
-        <v>250</v>
+        <v>237</v>
       </c>
       <c r="H16" s="31" t="s">
         <v>62</v>
@@ -3041,13 +3038,13 @@
         <v>61</v>
       </c>
       <c r="O16" s="31" t="s">
-        <v>251</v>
+        <v>238</v>
       </c>
       <c r="P16" s="33"/>
     </row>
     <row r="17" spans="1:16" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="33" t="s">
-        <v>252</v>
+        <v>239</v>
       </c>
       <c r="B17" s="39">
         <f>-0.07</f>
@@ -3064,7 +3061,7 @@
         <v>61</v>
       </c>
       <c r="G17" s="31" t="s">
-        <v>280</v>
+        <v>267</v>
       </c>
       <c r="H17" s="31" t="s">
         <v>62</v>
@@ -3088,7 +3085,7 @@
         <v>61</v>
       </c>
       <c r="O17" s="31" t="s">
-        <v>253</v>
+        <v>240</v>
       </c>
       <c r="P17" s="33"/>
     </row>
@@ -3103,7 +3100,7 @@
   <dimension ref="A1:P19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3134,7 +3131,7 @@
         <v>39</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="15"/>
@@ -3152,7 +3149,7 @@
         <v>42</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="15"/>
@@ -3254,7 +3251,7 @@
     </row>
     <row r="12" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="26" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="B12" s="27">
         <v>-1</v>
@@ -3264,7 +3261,7 @@
       </c>
       <c r="D12" s="20"/>
       <c r="E12" s="20" t="s">
-        <v>91</v>
+        <v>268</v>
       </c>
       <c r="F12" s="20" t="s">
         <v>61</v>
@@ -3294,7 +3291,7 @@
         <v>61</v>
       </c>
       <c r="O12" s="20" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="P12" s="26"/>
     </row>
@@ -3309,7 +3306,7 @@
         <v>84</v>
       </c>
       <c r="D13" s="31" t="s">
-        <v>201</v>
+        <v>274</v>
       </c>
       <c r="E13" s="31" t="s">
         <v>60</v>
@@ -3348,7 +3345,7 @@
     </row>
     <row r="14" spans="1:16" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="33" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="B14" s="34">
         <v>-1</v>
@@ -3358,7 +3355,7 @@
       </c>
       <c r="D14" s="31"/>
       <c r="E14" s="31" t="s">
-        <v>91</v>
+        <v>268</v>
       </c>
       <c r="F14" s="31" t="s">
         <v>61</v>
@@ -3388,7 +3385,7 @@
         <v>61</v>
       </c>
       <c r="O14" s="31" t="s">
-        <v>255</v>
+        <v>242</v>
       </c>
       <c r="P14" s="33"/>
     </row>
@@ -3493,7 +3490,7 @@
   <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3521,7 +3518,7 @@
         <v>39</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="15"/>
@@ -3539,7 +3536,7 @@
         <v>42</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="15"/>
@@ -3641,7 +3638,7 @@
     </row>
     <row r="12" spans="1:16" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="26" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="B12" s="27">
         <v>-1</v>
@@ -3651,7 +3648,7 @@
       </c>
       <c r="D12" s="20"/>
       <c r="E12" s="20" t="s">
-        <v>91</v>
+        <v>268</v>
       </c>
       <c r="F12" s="20" t="s">
         <v>61</v>
@@ -3681,13 +3678,13 @@
         <v>61</v>
       </c>
       <c r="O12" s="20" t="s">
-        <v>255</v>
+        <v>242</v>
       </c>
       <c r="P12" s="33"/>
     </row>
     <row r="13" spans="1:16" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="33" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B13" s="34">
         <v>-3.6</v>
@@ -3703,7 +3700,7 @@
         <v>61</v>
       </c>
       <c r="G13" s="31" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H13" s="31" t="s">
         <v>62</v>
@@ -3727,13 +3724,13 @@
         <v>61</v>
       </c>
       <c r="O13" s="31" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="P13" s="33"/>
     </row>
     <row r="14" spans="1:16" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="33" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B14" s="40">
         <v>0</v>
@@ -3742,7 +3739,7 @@
         <v>48</v>
       </c>
       <c r="D14" s="41" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E14" s="31" t="s">
         <v>60</v>
@@ -3751,7 +3748,7 @@
         <v>61</v>
       </c>
       <c r="G14" s="31" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H14" s="31" t="s">
         <v>62</v>
@@ -3775,13 +3772,13 @@
         <v>61</v>
       </c>
       <c r="O14" s="31" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="P14" s="33"/>
     </row>
     <row r="15" spans="1:16" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="33" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B15" s="40">
         <v>0</v>
@@ -3790,14 +3787,14 @@
         <v>48</v>
       </c>
       <c r="D15" s="41" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E15" s="31" t="s">
         <v>60</v>
       </c>
       <c r="F15" s="31"/>
       <c r="G15" s="31" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H15" s="31" t="s">
         <v>62</v>
@@ -3821,13 +3818,13 @@
         <v>61</v>
       </c>
       <c r="O15" s="31" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="P15" s="33"/>
     </row>
     <row r="16" spans="1:16" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="33" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B16" s="39">
         <f>-Hypothesis!D42</f>
@@ -3838,7 +3835,7 @@
       </c>
       <c r="D16" s="31"/>
       <c r="E16" s="31" t="s">
-        <v>91</v>
+        <v>268</v>
       </c>
       <c r="F16" s="31" t="s">
         <v>61</v>
@@ -3868,7 +3865,7 @@
         <v>61</v>
       </c>
       <c r="O16" s="31" t="s">
-        <v>256</v>
+        <v>243</v>
       </c>
       <c r="P16" s="33"/>
     </row>
@@ -3883,7 +3880,7 @@
   <dimension ref="A1:P19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3914,7 +3911,7 @@
         <v>39</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="15"/>
@@ -3932,7 +3929,7 @@
         <v>42</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="15"/>
@@ -4034,7 +4031,7 @@
     </row>
     <row r="12" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="26" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B12" s="27">
         <v>-1</v>
@@ -4044,7 +4041,7 @@
       </c>
       <c r="D12" s="20"/>
       <c r="E12" s="20" t="s">
-        <v>91</v>
+        <v>268</v>
       </c>
       <c r="F12" s="20" t="s">
         <v>61</v>
@@ -4074,7 +4071,7 @@
         <v>61</v>
       </c>
       <c r="O12" s="20" t="s">
-        <v>266</v>
+        <v>253</v>
       </c>
       <c r="P12" s="26"/>
     </row>
@@ -4089,7 +4086,7 @@
         <v>84</v>
       </c>
       <c r="D13" s="31" t="s">
-        <v>187</v>
+        <v>273</v>
       </c>
       <c r="E13" s="31" t="s">
         <v>60</v>
@@ -4128,7 +4125,7 @@
     </row>
     <row r="14" spans="1:16" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="33" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B14" s="34">
         <v>-1</v>
@@ -4138,7 +4135,7 @@
       </c>
       <c r="D14" s="31"/>
       <c r="E14" s="31" t="s">
-        <v>91</v>
+        <v>268</v>
       </c>
       <c r="F14" s="31" t="s">
         <v>61</v>
@@ -4168,7 +4165,7 @@
         <v>61</v>
       </c>
       <c r="O14" s="31" t="s">
-        <v>267</v>
+        <v>254</v>
       </c>
       <c r="P14" s="33"/>
     </row>
@@ -4301,7 +4298,7 @@
         <v>39</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="15"/>
@@ -4319,7 +4316,7 @@
         <v>42</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="15"/>
@@ -4421,7 +4418,7 @@
     </row>
     <row r="12" spans="1:16" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="26" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B12" s="27">
         <v>-1</v>
@@ -4431,7 +4428,7 @@
       </c>
       <c r="D12" s="20"/>
       <c r="E12" s="20" t="s">
-        <v>91</v>
+        <v>268</v>
       </c>
       <c r="F12" s="20" t="s">
         <v>61</v>
@@ -4461,13 +4458,13 @@
         <v>61</v>
       </c>
       <c r="O12" s="20" t="s">
-        <v>267</v>
+        <v>254</v>
       </c>
       <c r="P12" s="33"/>
     </row>
     <row r="13" spans="1:16" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="33" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B13" s="34">
         <v>-3.6</v>
@@ -4483,7 +4480,7 @@
         <v>61</v>
       </c>
       <c r="G13" s="31" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H13" s="31" t="s">
         <v>62</v>
@@ -4507,13 +4504,13 @@
         <v>61</v>
       </c>
       <c r="O13" s="31" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="P13" s="33"/>
     </row>
     <row r="14" spans="1:16" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="33" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B14" s="40">
         <v>0</v>
@@ -4522,7 +4519,7 @@
         <v>48</v>
       </c>
       <c r="D14" s="41" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E14" s="31" t="s">
         <v>60</v>
@@ -4531,7 +4528,7 @@
         <v>61</v>
       </c>
       <c r="G14" s="31" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H14" s="31" t="s">
         <v>62</v>
@@ -4555,13 +4552,13 @@
         <v>61</v>
       </c>
       <c r="O14" s="31" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="P14" s="33"/>
     </row>
     <row r="15" spans="1:16" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="33" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B15" s="40">
         <v>0</v>
@@ -4570,14 +4567,14 @@
         <v>48</v>
       </c>
       <c r="D15" s="41" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E15" s="31" t="s">
         <v>60</v>
       </c>
       <c r="F15" s="31"/>
       <c r="G15" s="31" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H15" s="31" t="s">
         <v>62</v>
@@ -4601,13 +4598,13 @@
         <v>61</v>
       </c>
       <c r="O15" s="31" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="P15" s="33"/>
     </row>
     <row r="16" spans="1:16" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="33" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B16" s="39">
         <f>-Hypothesis!D42</f>
@@ -4618,7 +4615,7 @@
       </c>
       <c r="D16" s="31"/>
       <c r="E16" s="31" t="s">
-        <v>91</v>
+        <v>268</v>
       </c>
       <c r="F16" s="31" t="s">
         <v>61</v>
@@ -4648,7 +4645,7 @@
         <v>61</v>
       </c>
       <c r="O16" s="31" t="s">
-        <v>258</v>
+        <v>245</v>
       </c>
       <c r="P16" s="33"/>
     </row>
@@ -4663,7 +4660,7 @@
   <dimension ref="A1:P19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4694,7 +4691,7 @@
         <v>39</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="15"/>
@@ -4712,7 +4709,7 @@
         <v>42</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="15"/>
@@ -4814,7 +4811,7 @@
     </row>
     <row r="12" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="26" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B12" s="27">
         <v>-1</v>
@@ -4824,7 +4821,7 @@
       </c>
       <c r="D12" s="20"/>
       <c r="E12" s="20" t="s">
-        <v>91</v>
+        <v>268</v>
       </c>
       <c r="F12" s="20" t="s">
         <v>61</v>
@@ -4854,7 +4851,7 @@
         <v>61</v>
       </c>
       <c r="O12" s="20" t="s">
-        <v>268</v>
+        <v>255</v>
       </c>
       <c r="P12" s="26"/>
     </row>
@@ -4869,7 +4866,7 @@
         <v>84</v>
       </c>
       <c r="D13" s="31" t="s">
-        <v>187</v>
+        <v>273</v>
       </c>
       <c r="E13" s="31" t="s">
         <v>60</v>
@@ -4908,7 +4905,7 @@
     </row>
     <row r="14" spans="1:16" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="33" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B14" s="34">
         <v>-1</v>
@@ -4918,7 +4915,7 @@
       </c>
       <c r="D14" s="31"/>
       <c r="E14" s="31" t="s">
-        <v>91</v>
+        <v>268</v>
       </c>
       <c r="F14" s="31" t="s">
         <v>61</v>
@@ -4948,7 +4945,7 @@
         <v>61</v>
       </c>
       <c r="O14" s="31" t="s">
-        <v>269</v>
+        <v>256</v>
       </c>
       <c r="P14" s="33"/>
     </row>
@@ -5052,8 +5049,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0858D22D-8E42-4544-AEDF-1AF1C1770151}">
   <dimension ref="A1:P16"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="O17" sqref="O17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5081,7 +5078,7 @@
         <v>39</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="15"/>
@@ -5099,7 +5096,7 @@
         <v>42</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="15"/>
@@ -5201,7 +5198,7 @@
     </row>
     <row r="12" spans="1:16" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="26" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B12" s="27">
         <v>-1</v>
@@ -5211,7 +5208,7 @@
       </c>
       <c r="D12" s="20"/>
       <c r="E12" s="20" t="s">
-        <v>91</v>
+        <v>268</v>
       </c>
       <c r="F12" s="20" t="s">
         <v>61</v>
@@ -5241,13 +5238,13 @@
         <v>61</v>
       </c>
       <c r="O12" s="20" t="s">
-        <v>269</v>
+        <v>256</v>
       </c>
       <c r="P12" s="33"/>
     </row>
     <row r="13" spans="1:16" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="33" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B13" s="34">
         <v>-3.6</v>
@@ -5263,7 +5260,7 @@
         <v>61</v>
       </c>
       <c r="G13" s="31" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H13" s="31" t="s">
         <v>62</v>
@@ -5287,13 +5284,13 @@
         <v>61</v>
       </c>
       <c r="O13" s="31" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="P13" s="33"/>
     </row>
     <row r="14" spans="1:16" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="33" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B14" s="40">
         <v>0</v>
@@ -5302,7 +5299,7 @@
         <v>48</v>
       </c>
       <c r="D14" s="41" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E14" s="31" t="s">
         <v>60</v>
@@ -5311,7 +5308,7 @@
         <v>61</v>
       </c>
       <c r="G14" s="31" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H14" s="31" t="s">
         <v>62</v>
@@ -5335,13 +5332,13 @@
         <v>61</v>
       </c>
       <c r="O14" s="31" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="P14" s="33"/>
     </row>
     <row r="15" spans="1:16" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="33" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B15" s="40">
         <v>0</v>
@@ -5350,14 +5347,14 @@
         <v>48</v>
       </c>
       <c r="D15" s="41" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E15" s="31" t="s">
         <v>60</v>
       </c>
       <c r="F15" s="31"/>
       <c r="G15" s="31" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H15" s="31" t="s">
         <v>62</v>
@@ -5381,13 +5378,13 @@
         <v>61</v>
       </c>
       <c r="O15" s="31" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="P15" s="33"/>
     </row>
     <row r="16" spans="1:16" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="33" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B16" s="39">
         <f>-Hypothesis!D42</f>
@@ -5398,7 +5395,7 @@
       </c>
       <c r="D16" s="31"/>
       <c r="E16" s="31" t="s">
-        <v>91</v>
+        <v>268</v>
       </c>
       <c r="F16" s="31" t="s">
         <v>61</v>
@@ -5428,7 +5425,7 @@
         <v>61</v>
       </c>
       <c r="O16" s="31" t="s">
-        <v>258</v>
+        <v>245</v>
       </c>
       <c r="P16" s="33"/>
     </row>
@@ -5443,7 +5440,7 @@
   <dimension ref="A1:P19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5474,7 +5471,7 @@
         <v>39</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="15"/>
@@ -5492,7 +5489,7 @@
         <v>42</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="15"/>
@@ -5594,7 +5591,7 @@
     </row>
     <row r="12" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="26" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="B12" s="27">
         <v>-1</v>
@@ -5604,7 +5601,7 @@
       </c>
       <c r="D12" s="20"/>
       <c r="E12" s="20" t="s">
-        <v>91</v>
+        <v>268</v>
       </c>
       <c r="F12" s="20" t="s">
         <v>61</v>
@@ -5634,7 +5631,7 @@
         <v>61</v>
       </c>
       <c r="O12" s="20" t="s">
-        <v>270</v>
+        <v>257</v>
       </c>
       <c r="P12" s="26"/>
     </row>
@@ -5649,7 +5646,7 @@
         <v>84</v>
       </c>
       <c r="D13" s="31" t="s">
-        <v>188</v>
+        <v>272</v>
       </c>
       <c r="E13" s="31" t="s">
         <v>60</v>
@@ -5688,7 +5685,7 @@
     </row>
     <row r="14" spans="1:16" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="33" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="B14" s="34">
         <v>-1</v>
@@ -5698,7 +5695,7 @@
       </c>
       <c r="D14" s="31"/>
       <c r="E14" s="31" t="s">
-        <v>91</v>
+        <v>268</v>
       </c>
       <c r="F14" s="31" t="s">
         <v>61</v>
@@ -5728,7 +5725,7 @@
         <v>61</v>
       </c>
       <c r="O14" s="31" t="s">
-        <v>271</v>
+        <v>258</v>
       </c>
       <c r="P14" s="33"/>
     </row>
@@ -5832,7 +5829,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D9A13F8-BDDC-47F8-8D17-F6340F6E3251}">
   <dimension ref="A1:P16"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
@@ -5861,7 +5858,7 @@
         <v>39</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="15"/>
@@ -5879,7 +5876,7 @@
         <v>42</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="15"/>
@@ -5981,7 +5978,7 @@
     </row>
     <row r="12" spans="1:16" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="26" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="B12" s="27">
         <v>-1</v>
@@ -5991,7 +5988,7 @@
       </c>
       <c r="D12" s="20"/>
       <c r="E12" s="20" t="s">
-        <v>91</v>
+        <v>268</v>
       </c>
       <c r="F12" s="20" t="s">
         <v>61</v>
@@ -6021,13 +6018,13 @@
         <v>61</v>
       </c>
       <c r="O12" s="20" t="s">
-        <v>271</v>
+        <v>258</v>
       </c>
       <c r="P12" s="33"/>
     </row>
     <row r="13" spans="1:16" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="33" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B13" s="34">
         <v>-3.6</v>
@@ -6043,7 +6040,7 @@
         <v>61</v>
       </c>
       <c r="G13" s="31" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H13" s="31" t="s">
         <v>62</v>
@@ -6067,13 +6064,13 @@
         <v>61</v>
       </c>
       <c r="O13" s="31" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="P13" s="33"/>
     </row>
     <row r="14" spans="1:16" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="33" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B14" s="40">
         <v>0</v>
@@ -6082,7 +6079,7 @@
         <v>48</v>
       </c>
       <c r="D14" s="41" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="E14" s="31" t="s">
         <v>60</v>
@@ -6091,7 +6088,7 @@
         <v>61</v>
       </c>
       <c r="G14" s="31" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H14" s="31" t="s">
         <v>62</v>
@@ -6115,13 +6112,13 @@
         <v>61</v>
       </c>
       <c r="O14" s="31" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="P14" s="33"/>
     </row>
     <row r="15" spans="1:16" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="33" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B15" s="40">
         <v>0</v>
@@ -6130,14 +6127,14 @@
         <v>48</v>
       </c>
       <c r="D15" s="41" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="E15" s="31" t="s">
         <v>60</v>
       </c>
       <c r="F15" s="31"/>
       <c r="G15" s="31" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H15" s="31" t="s">
         <v>62</v>
@@ -6161,13 +6158,13 @@
         <v>61</v>
       </c>
       <c r="O15" s="31" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="P15" s="33"/>
     </row>
     <row r="16" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="26" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B16" s="19">
         <f>-Hypothesis!D42</f>
@@ -6178,7 +6175,7 @@
       </c>
       <c r="D16" s="20"/>
       <c r="E16" s="20" t="s">
-        <v>91</v>
+        <v>268</v>
       </c>
       <c r="F16" s="20" t="s">
         <v>61</v>
@@ -6208,7 +6205,7 @@
         <v>61</v>
       </c>
       <c r="O16" s="20" t="s">
-        <v>260</v>
+        <v>247</v>
       </c>
       <c r="P16" s="26"/>
     </row>
@@ -6222,8 +6219,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64C8692C-E0F3-49D7-94C6-AE0594B1B749}">
   <dimension ref="A1:P53"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6231,7 +6228,7 @@
     <col min="1" max="1" width="65.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33.140625" customWidth="1"/>
     <col min="3" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="4" width="24.140625" customWidth="1"/>
+    <col min="4" max="4" width="65.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.5703125" customWidth="1"/>
     <col min="6" max="13" width="18.140625" customWidth="1"/>
     <col min="14" max="14" width="37.42578125" bestFit="1" customWidth="1"/>
@@ -6254,7 +6251,7 @@
         <v>32</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>91</v>
+        <v>268</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>33</v>
@@ -6340,7 +6337,7 @@
     </row>
     <row r="10" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B10" t="s">
         <v>13</v>
@@ -6349,15 +6346,15 @@
         <v>0</v>
       </c>
       <c r="D10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="11" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>13</v>
@@ -6367,12 +6364,12 @@
         <v>3.3115500000000009</v>
       </c>
       <c r="E11" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="12" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B12" s="8" t="s">
         <v>13</v>
@@ -6382,12 +6379,12 @@
         <v>0.09</v>
       </c>
       <c r="E12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="13" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B13" s="8" t="s">
         <v>13</v>
@@ -6397,12 +6394,12 @@
         <v>0.15</v>
       </c>
       <c r="E13" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="14" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B14" s="8" t="s">
         <v>13</v>
@@ -6412,12 +6409,12 @@
         <v>0.54749999999999999</v>
       </c>
       <c r="E14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B15" t="s">
         <v>13</v>
@@ -6426,16 +6423,16 @@
         <v>0</v>
       </c>
       <c r="D15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="O15"/>
     </row>
     <row r="16" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>13</v>
@@ -6445,12 +6442,12 @@
         <v>3.4749000000000008</v>
       </c>
       <c r="E16" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="17" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B17" s="8" t="s">
         <v>13</v>
@@ -6460,12 +6457,12 @@
         <v>0.09</v>
       </c>
       <c r="E17" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="18" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B18" s="8" t="s">
         <v>13</v>
@@ -6475,12 +6472,12 @@
         <v>0.15</v>
       </c>
       <c r="E18" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="19" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B19" s="8" t="s">
         <v>13</v>
@@ -6490,12 +6487,12 @@
         <v>0.67499999999999993</v>
       </c>
       <c r="E19" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B20" t="s">
         <v>13</v>
@@ -6504,16 +6501,16 @@
         <v>0</v>
       </c>
       <c r="D20" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E20" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="O20"/>
     </row>
     <row r="21" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B21" s="8" t="s">
         <v>13</v>
@@ -6523,12 +6520,12 @@
         <v>3.7867500000000005</v>
       </c>
       <c r="E21" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="22" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B22" s="8" t="s">
         <v>13</v>
@@ -6538,12 +6535,12 @@
         <v>0.77999999999999992</v>
       </c>
       <c r="E22" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B23" t="s">
         <v>13</v>
@@ -6552,16 +6549,16 @@
         <v>0</v>
       </c>
       <c r="D23" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E23" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="O23"/>
     </row>
     <row r="24" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B24" s="8" t="s">
         <v>13</v>
@@ -6571,12 +6568,12 @@
         <v>13.216500000000002</v>
       </c>
       <c r="E24" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="25" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B25" s="8" t="s">
         <v>13</v>
@@ -6586,12 +6583,12 @@
         <v>1.95</v>
       </c>
       <c r="E25" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B26" t="s">
         <v>13</v>
@@ -6600,16 +6597,16 @@
         <v>0</v>
       </c>
       <c r="D26" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E26" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="O26"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B27" t="s">
         <v>13</v>
@@ -6618,16 +6615,16 @@
         <v>0</v>
       </c>
       <c r="D27" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E27" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="O27"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="B28" t="s">
         <v>13</v>
@@ -6636,13 +6633,13 @@
         <v>0.94</v>
       </c>
       <c r="E28" t="s">
-        <v>241</v>
+        <v>231</v>
       </c>
       <c r="O28"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B29" t="s">
         <v>13</v>
@@ -6651,16 +6648,16 @@
         <v>0</v>
       </c>
       <c r="D29" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E29" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="O29"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B30" t="s">
         <v>13</v>
@@ -6670,13 +6667,13 @@
         <v>6.7864500000000021</v>
       </c>
       <c r="E30" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="O30"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B31" t="s">
         <v>13</v>
@@ -6686,37 +6683,37 @@
         <v>1.2224999999999999</v>
       </c>
       <c r="E31" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="O31"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B32" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C32" s="37">
         <v>130</v>
       </c>
       <c r="E32" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="O32"/>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B33" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C33" s="37">
         <v>50</v>
       </c>
       <c r="E33" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="O33"/>
     </row>
@@ -6732,7 +6729,7 @@
         <v>39</v>
       </c>
       <c r="B36" s="14" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C36" s="4"/>
       <c r="D36" s="15"/>
@@ -6750,7 +6747,7 @@
         <v>42</v>
       </c>
       <c r="B38" s="16" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="C38" s="4"/>
       <c r="D38" s="15"/>
@@ -6852,7 +6849,7 @@
     </row>
     <row r="46" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="26" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B46" s="27">
         <v>-1</v>
@@ -6862,7 +6859,7 @@
       </c>
       <c r="D46" s="20"/>
       <c r="E46" s="20" t="s">
-        <v>91</v>
+        <v>268</v>
       </c>
       <c r="F46" s="20" t="s">
         <v>61</v>
@@ -6892,7 +6889,7 @@
         <v>61</v>
       </c>
       <c r="O46" s="20" t="s">
-        <v>256</v>
+        <v>243</v>
       </c>
       <c r="P46" s="26"/>
     </row>
@@ -6907,7 +6904,7 @@
         <v>84</v>
       </c>
       <c r="D47" s="31" t="s">
-        <v>184</v>
+        <v>279</v>
       </c>
       <c r="E47" s="31" t="s">
         <v>60</v>
@@ -6946,7 +6943,7 @@
     </row>
     <row r="48" spans="1:16" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="33" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B48" s="34">
         <v>-1</v>
@@ -6956,7 +6953,7 @@
       </c>
       <c r="D48" s="31"/>
       <c r="E48" s="31" t="s">
-        <v>91</v>
+        <v>268</v>
       </c>
       <c r="F48" s="31" t="s">
         <v>61</v>
@@ -6986,7 +6983,7 @@
         <v>61</v>
       </c>
       <c r="O48" s="31" t="s">
-        <v>257</v>
+        <v>244</v>
       </c>
       <c r="P48" s="33"/>
     </row>
@@ -7091,7 +7088,7 @@
   <dimension ref="A1:P19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7122,7 +7119,7 @@
         <v>39</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="15"/>
@@ -7140,7 +7137,7 @@
         <v>42</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="15"/>
@@ -7242,7 +7239,7 @@
     </row>
     <row r="12" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="26" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="B12" s="27">
         <v>-1</v>
@@ -7252,7 +7249,7 @@
       </c>
       <c r="D12" s="20"/>
       <c r="E12" s="20" t="s">
-        <v>91</v>
+        <v>268</v>
       </c>
       <c r="F12" s="20" t="s">
         <v>61</v>
@@ -7282,7 +7279,7 @@
         <v>61</v>
       </c>
       <c r="O12" s="20" t="s">
-        <v>272</v>
+        <v>259</v>
       </c>
       <c r="P12" s="26"/>
     </row>
@@ -7297,7 +7294,7 @@
         <v>84</v>
       </c>
       <c r="D13" s="31" t="s">
-        <v>196</v>
+        <v>269</v>
       </c>
       <c r="E13" s="31" t="s">
         <v>60</v>
@@ -7336,7 +7333,7 @@
     </row>
     <row r="14" spans="1:16" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="33" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="B14" s="34">
         <v>-1</v>
@@ -7346,7 +7343,7 @@
       </c>
       <c r="D14" s="31"/>
       <c r="E14" s="31" t="s">
-        <v>91</v>
+        <v>268</v>
       </c>
       <c r="F14" s="31" t="s">
         <v>61</v>
@@ -7376,7 +7373,7 @@
         <v>61</v>
       </c>
       <c r="O14" s="31" t="s">
-        <v>273</v>
+        <v>260</v>
       </c>
       <c r="P14" s="33"/>
     </row>
@@ -7509,7 +7506,7 @@
         <v>39</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="15"/>
@@ -7527,7 +7524,7 @@
         <v>42</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="15"/>
@@ -7629,7 +7626,7 @@
     </row>
     <row r="12" spans="1:16" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="26" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="B12" s="27">
         <v>-1</v>
@@ -7639,7 +7636,7 @@
       </c>
       <c r="D12" s="20"/>
       <c r="E12" s="20" t="s">
-        <v>91</v>
+        <v>268</v>
       </c>
       <c r="F12" s="20" t="s">
         <v>61</v>
@@ -7669,13 +7666,13 @@
         <v>61</v>
       </c>
       <c r="O12" s="20" t="s">
-        <v>273</v>
+        <v>260</v>
       </c>
       <c r="P12" s="33"/>
     </row>
     <row r="13" spans="1:16" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="33" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B13" s="34">
         <v>-4.4000000000000004</v>
@@ -7691,7 +7688,7 @@
         <v>61</v>
       </c>
       <c r="G13" s="31" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H13" s="31" t="s">
         <v>62</v>
@@ -7715,13 +7712,13 @@
         <v>61</v>
       </c>
       <c r="O13" s="31" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="P13" s="33"/>
     </row>
     <row r="14" spans="1:16" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="33" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B14" s="40">
         <v>0</v>
@@ -7730,7 +7727,7 @@
         <v>48</v>
       </c>
       <c r="D14" s="41" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="E14" s="31" t="s">
         <v>60</v>
@@ -7739,7 +7736,7 @@
         <v>61</v>
       </c>
       <c r="G14" s="31" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H14" s="31" t="s">
         <v>62</v>
@@ -7763,13 +7760,13 @@
         <v>61</v>
       </c>
       <c r="O14" s="31" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="P14" s="33"/>
     </row>
     <row r="15" spans="1:16" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="33" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B15" s="40">
         <v>0</v>
@@ -7778,14 +7775,14 @@
         <v>48</v>
       </c>
       <c r="D15" s="41" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="E15" s="31" t="s">
         <v>60</v>
       </c>
       <c r="F15" s="31"/>
       <c r="G15" s="31" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H15" s="31" t="s">
         <v>62</v>
@@ -7809,13 +7806,13 @@
         <v>61</v>
       </c>
       <c r="O15" s="31" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="P15" s="33"/>
     </row>
     <row r="16" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="26" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B16" s="19">
         <f>-Hypothesis!D42</f>
@@ -7826,7 +7823,7 @@
       </c>
       <c r="D16" s="20"/>
       <c r="E16" s="20" t="s">
-        <v>91</v>
+        <v>268</v>
       </c>
       <c r="F16" s="20" t="s">
         <v>61</v>
@@ -7856,13 +7853,13 @@
         <v>61</v>
       </c>
       <c r="O16" s="20" t="s">
-        <v>258</v>
+        <v>245</v>
       </c>
       <c r="P16" s="26"/>
     </row>
     <row r="17" spans="1:15" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B17" s="19">
         <f>-Hypothesis!D42</f>
@@ -7873,7 +7870,7 @@
       </c>
       <c r="D17" s="20"/>
       <c r="E17" s="20" t="s">
-        <v>91</v>
+        <v>268</v>
       </c>
       <c r="F17" s="20" t="s">
         <v>61</v>
@@ -7903,7 +7900,7 @@
         <v>61</v>
       </c>
       <c r="O17" s="20" t="s">
-        <v>256</v>
+        <v>243</v>
       </c>
     </row>
   </sheetData>
@@ -7917,7 +7914,7 @@
   <dimension ref="A1:P19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7948,7 +7945,7 @@
         <v>39</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="15"/>
@@ -7966,7 +7963,7 @@
         <v>42</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="15"/>
@@ -8068,7 +8065,7 @@
     </row>
     <row r="12" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="26" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="B12" s="27">
         <v>-1</v>
@@ -8078,7 +8075,7 @@
       </c>
       <c r="D12" s="20"/>
       <c r="E12" s="20" t="s">
-        <v>91</v>
+        <v>268</v>
       </c>
       <c r="F12" s="20" t="s">
         <v>61</v>
@@ -8108,7 +8105,7 @@
         <v>61</v>
       </c>
       <c r="O12" s="20" t="s">
-        <v>274</v>
+        <v>261</v>
       </c>
       <c r="P12" s="26"/>
     </row>
@@ -8123,7 +8120,7 @@
         <v>84</v>
       </c>
       <c r="D13" s="31" t="s">
-        <v>209</v>
+        <v>271</v>
       </c>
       <c r="E13" s="31" t="s">
         <v>60</v>
@@ -8162,7 +8159,7 @@
     </row>
     <row r="14" spans="1:16" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="33" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="B14" s="34">
         <v>-1</v>
@@ -8172,7 +8169,7 @@
       </c>
       <c r="D14" s="31"/>
       <c r="E14" s="31" t="s">
-        <v>91</v>
+        <v>268</v>
       </c>
       <c r="F14" s="31" t="s">
         <v>61</v>
@@ -8202,7 +8199,7 @@
         <v>61</v>
       </c>
       <c r="O14" s="31" t="s">
-        <v>275</v>
+        <v>262</v>
       </c>
       <c r="P14" s="33"/>
     </row>
@@ -8307,7 +8304,7 @@
   <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O17" sqref="O17"/>
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8335,7 +8332,7 @@
         <v>39</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="15"/>
@@ -8353,7 +8350,7 @@
         <v>42</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="15"/>
@@ -8455,7 +8452,7 @@
     </row>
     <row r="12" spans="1:16" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="26" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="B12" s="27">
         <v>-1</v>
@@ -8465,7 +8462,7 @@
       </c>
       <c r="D12" s="20"/>
       <c r="E12" s="20" t="s">
-        <v>91</v>
+        <v>268</v>
       </c>
       <c r="F12" s="20" t="s">
         <v>61</v>
@@ -8495,13 +8492,13 @@
         <v>61</v>
       </c>
       <c r="O12" s="20" t="s">
-        <v>275</v>
+        <v>262</v>
       </c>
       <c r="P12" s="33"/>
     </row>
     <row r="13" spans="1:16" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="33" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B13" s="34">
         <v>-4.4000000000000004</v>
@@ -8517,7 +8514,7 @@
         <v>61</v>
       </c>
       <c r="G13" s="31" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H13" s="31" t="s">
         <v>62</v>
@@ -8541,13 +8538,13 @@
         <v>61</v>
       </c>
       <c r="O13" s="31" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="P13" s="33"/>
     </row>
     <row r="14" spans="1:16" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="33" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B14" s="40">
         <v>0</v>
@@ -8556,7 +8553,7 @@
         <v>48</v>
       </c>
       <c r="D14" s="41" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="E14" s="31" t="s">
         <v>60</v>
@@ -8565,7 +8562,7 @@
         <v>61</v>
       </c>
       <c r="G14" s="31" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H14" s="31" t="s">
         <v>62</v>
@@ -8589,13 +8586,13 @@
         <v>61</v>
       </c>
       <c r="O14" s="31" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="P14" s="33"/>
     </row>
     <row r="15" spans="1:16" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="33" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B15" s="40">
         <v>0</v>
@@ -8604,14 +8601,14 @@
         <v>48</v>
       </c>
       <c r="D15" s="41" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="E15" s="31" t="s">
         <v>60</v>
       </c>
       <c r="F15" s="31"/>
       <c r="G15" s="31" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H15" s="31" t="s">
         <v>62</v>
@@ -8635,13 +8632,13 @@
         <v>61</v>
       </c>
       <c r="O15" s="31" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="P15" s="33"/>
     </row>
     <row r="16" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="26" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="B16" s="19">
         <f>-Hypothesis!D42</f>
@@ -8652,7 +8649,7 @@
       </c>
       <c r="D16" s="20"/>
       <c r="E16" s="20" t="s">
-        <v>91</v>
+        <v>268</v>
       </c>
       <c r="F16" s="20" t="s">
         <v>61</v>
@@ -8682,7 +8679,7 @@
         <v>61</v>
       </c>
       <c r="O16" s="20" t="s">
-        <v>262</v>
+        <v>249</v>
       </c>
       <c r="P16" s="26"/>
     </row>
@@ -8697,7 +8694,7 @@
   <dimension ref="A1:P19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8728,7 +8725,7 @@
         <v>39</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="15"/>
@@ -8746,7 +8743,7 @@
         <v>42</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="15"/>
@@ -8848,7 +8845,7 @@
     </row>
     <row r="12" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="26" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
       <c r="B12" s="27">
         <v>-1</v>
@@ -8858,7 +8855,7 @@
       </c>
       <c r="D12" s="20"/>
       <c r="E12" s="20" t="s">
-        <v>91</v>
+        <v>268</v>
       </c>
       <c r="F12" s="20" t="s">
         <v>61</v>
@@ -8888,7 +8885,7 @@
         <v>61</v>
       </c>
       <c r="O12" s="20" t="s">
-        <v>276</v>
+        <v>263</v>
       </c>
       <c r="P12" s="26"/>
     </row>
@@ -8903,7 +8900,7 @@
         <v>84</v>
       </c>
       <c r="D13" s="31" t="s">
-        <v>242</v>
+        <v>270</v>
       </c>
       <c r="E13" s="31" t="s">
         <v>60</v>
@@ -8942,7 +8939,7 @@
     </row>
     <row r="14" spans="1:16" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="33" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
       <c r="B14" s="34">
         <v>-1</v>
@@ -8952,7 +8949,7 @@
       </c>
       <c r="D14" s="31"/>
       <c r="E14" s="31" t="s">
-        <v>91</v>
+        <v>268</v>
       </c>
       <c r="F14" s="31" t="s">
         <v>61</v>
@@ -8982,7 +8979,7 @@
         <v>61</v>
       </c>
       <c r="O14" s="31" t="s">
-        <v>277</v>
+        <v>264</v>
       </c>
       <c r="P14" s="33"/>
     </row>
@@ -9087,7 +9084,7 @@
   <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9115,7 +9112,7 @@
         <v>39</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="15"/>
@@ -9133,7 +9130,7 @@
         <v>42</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>238</v>
+        <v>228</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="15"/>
@@ -9235,7 +9232,7 @@
     </row>
     <row r="12" spans="1:16" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="26" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
       <c r="B12" s="27">
         <v>-1</v>
@@ -9245,7 +9242,7 @@
       </c>
       <c r="D12" s="20"/>
       <c r="E12" s="20" t="s">
-        <v>91</v>
+        <v>268</v>
       </c>
       <c r="F12" s="20" t="s">
         <v>61</v>
@@ -9275,13 +9272,13 @@
         <v>61</v>
       </c>
       <c r="O12" s="20" t="s">
-        <v>277</v>
+        <v>264</v>
       </c>
       <c r="P12" s="33"/>
     </row>
     <row r="13" spans="1:16" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="33" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B13" s="34">
         <v>-3.6</v>
@@ -9297,7 +9294,7 @@
         <v>61</v>
       </c>
       <c r="G13" s="31" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H13" s="31" t="s">
         <v>62</v>
@@ -9321,13 +9318,13 @@
         <v>61</v>
       </c>
       <c r="O13" s="31" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="P13" s="33"/>
     </row>
     <row r="14" spans="1:16" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="33" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B14" s="40">
         <v>0</v>
@@ -9336,7 +9333,7 @@
         <v>48</v>
       </c>
       <c r="D14" s="41" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E14" s="31" t="s">
         <v>60</v>
@@ -9345,7 +9342,7 @@
         <v>61</v>
       </c>
       <c r="G14" s="31" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H14" s="31" t="s">
         <v>62</v>
@@ -9369,13 +9366,13 @@
         <v>61</v>
       </c>
       <c r="O14" s="31" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="P14" s="33"/>
     </row>
     <row r="15" spans="1:16" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="33" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B15" s="40">
         <v>0</v>
@@ -9384,14 +9381,14 @@
         <v>48</v>
       </c>
       <c r="D15" s="41" t="s">
-        <v>243</v>
+        <v>181</v>
       </c>
       <c r="E15" s="31" t="s">
         <v>60</v>
       </c>
       <c r="F15" s="31"/>
       <c r="G15" s="31" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H15" s="31" t="s">
         <v>62</v>
@@ -9415,13 +9412,13 @@
         <v>61</v>
       </c>
       <c r="O15" s="31" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="P15" s="33"/>
     </row>
     <row r="16" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="26" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
       <c r="B16" s="19">
         <f>-Hypothesis!D42</f>
@@ -9432,7 +9429,7 @@
       </c>
       <c r="D16" s="20"/>
       <c r="E16" s="20" t="s">
-        <v>91</v>
+        <v>268</v>
       </c>
       <c r="F16" s="20" t="s">
         <v>61</v>
@@ -9462,7 +9459,7 @@
         <v>61</v>
       </c>
       <c r="O16" s="20" t="s">
-        <v>264</v>
+        <v>251</v>
       </c>
       <c r="P16" s="26"/>
     </row>
@@ -9477,7 +9474,7 @@
   <dimension ref="A1:P19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9508,7 +9505,7 @@
         <v>39</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="15"/>
@@ -9526,7 +9523,7 @@
         <v>42</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="15"/>
@@ -9628,7 +9625,7 @@
     </row>
     <row r="12" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="26" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="B12" s="27">
         <v>-1</v>
@@ -9638,7 +9635,7 @@
       </c>
       <c r="D12" s="20"/>
       <c r="E12" s="20" t="s">
-        <v>91</v>
+        <v>268</v>
       </c>
       <c r="F12" s="20" t="s">
         <v>61</v>
@@ -9668,7 +9665,7 @@
         <v>61</v>
       </c>
       <c r="O12" s="20" t="s">
-        <v>278</v>
+        <v>265</v>
       </c>
       <c r="P12" s="26"/>
     </row>
@@ -9683,7 +9680,7 @@
         <v>84</v>
       </c>
       <c r="D13" s="31" t="s">
-        <v>196</v>
+        <v>269</v>
       </c>
       <c r="E13" s="31" t="s">
         <v>60</v>
@@ -9722,7 +9719,7 @@
     </row>
     <row r="14" spans="1:16" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="33" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="B14" s="34">
         <v>-1</v>
@@ -9732,7 +9729,7 @@
       </c>
       <c r="D14" s="31"/>
       <c r="E14" s="31" t="s">
-        <v>91</v>
+        <v>268</v>
       </c>
       <c r="F14" s="31" t="s">
         <v>61</v>
@@ -9762,7 +9759,7 @@
         <v>61</v>
       </c>
       <c r="O14" s="31" t="s">
-        <v>279</v>
+        <v>266</v>
       </c>
       <c r="P14" s="33"/>
     </row>
@@ -9867,7 +9864,7 @@
   <dimension ref="A1:P17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9895,7 +9892,7 @@
         <v>39</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="15"/>
@@ -9913,7 +9910,7 @@
         <v>42</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="15"/>
@@ -10015,7 +10012,7 @@
     </row>
     <row r="12" spans="1:16" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="26" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="B12" s="27">
         <v>-1</v>
@@ -10025,7 +10022,7 @@
       </c>
       <c r="D12" s="20"/>
       <c r="E12" s="20" t="s">
-        <v>91</v>
+        <v>268</v>
       </c>
       <c r="F12" s="20" t="s">
         <v>61</v>
@@ -10055,13 +10052,13 @@
         <v>61</v>
       </c>
       <c r="O12" s="20" t="s">
-        <v>279</v>
+        <v>266</v>
       </c>
       <c r="P12" s="33"/>
     </row>
     <row r="13" spans="1:16" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="33" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B13" s="34">
         <v>-9.1</v>
@@ -10077,7 +10074,7 @@
         <v>61</v>
       </c>
       <c r="G13" s="31" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H13" s="31" t="s">
         <v>62</v>
@@ -10101,13 +10098,13 @@
         <v>61</v>
       </c>
       <c r="O13" s="31" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="P13" s="33"/>
     </row>
     <row r="14" spans="1:16" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="33" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B14" s="40">
         <v>0</v>
@@ -10116,7 +10113,7 @@
         <v>48</v>
       </c>
       <c r="D14" s="41" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="E14" s="31" t="s">
         <v>60</v>
@@ -10125,7 +10122,7 @@
         <v>61</v>
       </c>
       <c r="G14" s="31" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H14" s="31" t="s">
         <v>62</v>
@@ -10149,13 +10146,13 @@
         <v>61</v>
       </c>
       <c r="O14" s="31" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="P14" s="33"/>
     </row>
     <row r="15" spans="1:16" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="33" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B15" s="40">
         <v>0</v>
@@ -10164,7 +10161,7 @@
         <v>48</v>
       </c>
       <c r="D15" s="41" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="E15" s="31" t="s">
         <v>60</v>
@@ -10173,7 +10170,7 @@
         <v>61</v>
       </c>
       <c r="G15" s="31" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H15" s="31" t="s">
         <v>62</v>
@@ -10197,13 +10194,13 @@
         <v>61</v>
       </c>
       <c r="O15" s="31" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="P15" s="33"/>
     </row>
     <row r="16" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="26" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B16" s="19">
         <f>-Hypothesis!D42</f>
@@ -10214,7 +10211,7 @@
       </c>
       <c r="D16" s="20"/>
       <c r="E16" s="20" t="s">
-        <v>91</v>
+        <v>268</v>
       </c>
       <c r="F16" s="20" t="s">
         <v>61</v>
@@ -10244,13 +10241,13 @@
         <v>61</v>
       </c>
       <c r="O16" s="20" t="s">
-        <v>258</v>
+        <v>245</v>
       </c>
       <c r="P16" s="26"/>
     </row>
     <row r="17" spans="1:15" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B17" s="19">
         <f>-Hypothesis!D42</f>
@@ -10261,7 +10258,7 @@
       </c>
       <c r="D17" s="20"/>
       <c r="E17" s="20" t="s">
-        <v>91</v>
+        <v>268</v>
       </c>
       <c r="F17" s="20" t="s">
         <v>61</v>
@@ -10291,7 +10288,7 @@
         <v>61</v>
       </c>
       <c r="O17" s="20" t="s">
-        <v>256</v>
+        <v>243</v>
       </c>
     </row>
   </sheetData>
@@ -10336,7 +10333,7 @@
         <v>39</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="15"/>
@@ -10354,7 +10351,7 @@
         <v>42</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="15"/>
@@ -10456,7 +10453,7 @@
     </row>
     <row r="12" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="26" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B12" s="27">
         <v>-1</v>
@@ -10466,7 +10463,7 @@
       </c>
       <c r="D12" s="20"/>
       <c r="E12" s="20" t="s">
-        <v>91</v>
+        <v>268</v>
       </c>
       <c r="F12" s="20" t="s">
         <v>61</v>
@@ -10496,13 +10493,13 @@
         <v>61</v>
       </c>
       <c r="O12" s="20" t="s">
-        <v>257</v>
+        <v>244</v>
       </c>
       <c r="P12" s="26"/>
     </row>
     <row r="13" spans="1:16" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="33" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="B13" s="40">
         <v>0</v>
@@ -10511,7 +10508,7 @@
         <v>48</v>
       </c>
       <c r="D13" s="42" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E13" s="31" t="s">
         <v>60</v>
@@ -10520,7 +10517,7 @@
         <v>61</v>
       </c>
       <c r="G13" s="31" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H13" s="31" t="s">
         <v>62</v>
@@ -10544,7 +10541,7 @@
         <v>61</v>
       </c>
       <c r="O13" s="31" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="P13" s="33"/>
     </row>
@@ -10595,7 +10592,7 @@
   <dimension ref="A1:P19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10626,7 +10623,7 @@
         <v>39</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="15"/>
@@ -10644,7 +10641,7 @@
         <v>42</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="15"/>
@@ -10746,7 +10743,7 @@
     </row>
     <row r="12" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="26" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B12" s="27">
         <v>-1</v>
@@ -10756,7 +10753,7 @@
       </c>
       <c r="D12" s="20"/>
       <c r="E12" s="20" t="s">
-        <v>91</v>
+        <v>268</v>
       </c>
       <c r="F12" s="20" t="s">
         <v>61</v>
@@ -10786,7 +10783,7 @@
         <v>61</v>
       </c>
       <c r="O12" s="20" t="s">
-        <v>258</v>
+        <v>245</v>
       </c>
       <c r="P12" s="26"/>
     </row>
@@ -10801,7 +10798,7 @@
         <v>84</v>
       </c>
       <c r="D13" s="31" t="s">
-        <v>185</v>
+        <v>278</v>
       </c>
       <c r="E13" s="31" t="s">
         <v>60</v>
@@ -10840,7 +10837,7 @@
     </row>
     <row r="14" spans="1:16" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="33" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B14" s="34">
         <v>-1</v>
@@ -10850,7 +10847,7 @@
       </c>
       <c r="D14" s="31"/>
       <c r="E14" s="31" t="s">
-        <v>91</v>
+        <v>268</v>
       </c>
       <c r="F14" s="31" t="s">
         <v>61</v>
@@ -10880,7 +10877,7 @@
         <v>61</v>
       </c>
       <c r="O14" s="31" t="s">
-        <v>259</v>
+        <v>246</v>
       </c>
       <c r="P14" s="33"/>
     </row>
@@ -10984,7 +10981,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D18C70D-3BA6-4FA7-B2A5-397D5839FA4E}">
   <dimension ref="A1:P17"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
@@ -11016,7 +11013,7 @@
         <v>39</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="15"/>
@@ -11034,7 +11031,7 @@
         <v>42</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="15"/>
@@ -11136,7 +11133,7 @@
     </row>
     <row r="12" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="26" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B12" s="27">
         <v>-1</v>
@@ -11146,7 +11143,7 @@
       </c>
       <c r="D12" s="20"/>
       <c r="E12" s="20" t="s">
-        <v>91</v>
+        <v>268</v>
       </c>
       <c r="F12" s="20" t="s">
         <v>61</v>
@@ -11176,13 +11173,13 @@
         <v>61</v>
       </c>
       <c r="O12" s="20" t="s">
-        <v>259</v>
+        <v>246</v>
       </c>
       <c r="P12" s="26"/>
     </row>
     <row r="13" spans="1:16" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="33" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="B13" s="40">
         <v>0</v>
@@ -11191,7 +11188,7 @@
         <v>48</v>
       </c>
       <c r="D13" s="42" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E13" s="31" t="s">
         <v>60</v>
@@ -11200,7 +11197,7 @@
         <v>61</v>
       </c>
       <c r="G13" s="31" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H13" s="31" t="s">
         <v>62</v>
@@ -11224,13 +11221,13 @@
         <v>61</v>
       </c>
       <c r="O13" s="31" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="P13" s="33"/>
     </row>
     <row r="14" spans="1:16" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="33" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B14" s="34">
         <v>-0.15</v>
@@ -11246,7 +11243,7 @@
         <v>61</v>
       </c>
       <c r="G14" s="31" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H14" s="31" t="s">
         <v>62</v>
@@ -11270,13 +11267,13 @@
         <v>61</v>
       </c>
       <c r="O14" s="31" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="P14" s="33"/>
     </row>
     <row r="15" spans="1:16" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="33" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B15" s="39">
         <v>-0.04</v>
@@ -11292,7 +11289,7 @@
         <v>61</v>
       </c>
       <c r="G15" s="31" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H15" s="31" t="s">
         <v>62</v>
@@ -11316,10 +11313,10 @@
         <v>61</v>
       </c>
       <c r="O15" s="31" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="P15" s="33" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="35" customFormat="1" x14ac:dyDescent="0.25">
@@ -11369,7 +11366,7 @@
   <dimension ref="A1:P19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11402,7 +11399,7 @@
         <v>39</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="15"/>
@@ -11420,7 +11417,7 @@
         <v>42</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="15"/>
@@ -11522,7 +11519,7 @@
     </row>
     <row r="12" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="26" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B12" s="27">
         <v>-1</v>
@@ -11532,7 +11529,7 @@
       </c>
       <c r="D12" s="20"/>
       <c r="E12" s="20" t="s">
-        <v>91</v>
+        <v>268</v>
       </c>
       <c r="F12" s="20" t="s">
         <v>61</v>
@@ -11562,7 +11559,7 @@
         <v>61</v>
       </c>
       <c r="O12" s="20" t="s">
-        <v>260</v>
+        <v>247</v>
       </c>
       <c r="P12" s="26"/>
     </row>
@@ -11577,7 +11574,7 @@
         <v>84</v>
       </c>
       <c r="D13" s="31" t="s">
-        <v>186</v>
+        <v>277</v>
       </c>
       <c r="E13" s="31" t="s">
         <v>60</v>
@@ -11616,7 +11613,7 @@
     </row>
     <row r="14" spans="1:16" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="33" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B14" s="34">
         <v>-1</v>
@@ -11626,7 +11623,7 @@
       </c>
       <c r="D14" s="31"/>
       <c r="E14" s="31" t="s">
-        <v>91</v>
+        <v>268</v>
       </c>
       <c r="F14" s="31" t="s">
         <v>61</v>
@@ -11656,7 +11653,7 @@
         <v>61</v>
       </c>
       <c r="O14" s="31" t="s">
-        <v>261</v>
+        <v>248</v>
       </c>
       <c r="P14" s="33"/>
     </row>
@@ -11792,7 +11789,7 @@
         <v>39</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="15"/>
@@ -11810,7 +11807,7 @@
         <v>42</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="15"/>
@@ -11912,7 +11909,7 @@
     </row>
     <row r="12" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="26" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B12" s="27">
         <v>-1</v>
@@ -11922,7 +11919,7 @@
       </c>
       <c r="D12" s="20"/>
       <c r="E12" s="20" t="s">
-        <v>91</v>
+        <v>268</v>
       </c>
       <c r="F12" s="20" t="s">
         <v>61</v>
@@ -11952,13 +11949,13 @@
         <v>61</v>
       </c>
       <c r="O12" s="20" t="s">
-        <v>261</v>
+        <v>248</v>
       </c>
       <c r="P12" s="26"/>
     </row>
     <row r="13" spans="1:16" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="33" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="B13" s="40">
         <v>0</v>
@@ -11967,7 +11964,7 @@
         <v>48</v>
       </c>
       <c r="D13" s="42" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E13" s="31" t="s">
         <v>60</v>
@@ -11976,7 +11973,7 @@
         <v>61</v>
       </c>
       <c r="G13" s="31" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H13" s="31" t="s">
         <v>62</v>
@@ -12000,13 +11997,13 @@
         <v>61</v>
       </c>
       <c r="O13" s="31" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="P13" s="33"/>
     </row>
     <row r="14" spans="1:16" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="33" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B14" s="39">
         <f>-0.15*2</f>
@@ -12023,7 +12020,7 @@
         <v>61</v>
       </c>
       <c r="G14" s="31" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H14" s="31" t="s">
         <v>62</v>
@@ -12047,13 +12044,13 @@
         <v>61</v>
       </c>
       <c r="O14" s="31" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="P14" s="33"/>
     </row>
     <row r="15" spans="1:16" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="33" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B15" s="39">
         <f>-0.04*2</f>
@@ -12070,7 +12067,7 @@
         <v>61</v>
       </c>
       <c r="G15" s="31" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H15" s="31" t="s">
         <v>62</v>
@@ -12094,10 +12091,10 @@
         <v>61</v>
       </c>
       <c r="O15" s="31" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="P15" s="33" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="35" customFormat="1" x14ac:dyDescent="0.25">
@@ -12147,7 +12144,7 @@
   <dimension ref="A1:P19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12180,7 +12177,7 @@
         <v>39</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="15"/>
@@ -12198,7 +12195,7 @@
         <v>42</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="15"/>
@@ -12300,7 +12297,7 @@
     </row>
     <row r="12" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="26" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="B12" s="27">
         <v>-1</v>
@@ -12310,7 +12307,7 @@
       </c>
       <c r="D12" s="20"/>
       <c r="E12" s="20" t="s">
-        <v>91</v>
+        <v>268</v>
       </c>
       <c r="F12" s="20" t="s">
         <v>61</v>
@@ -12340,7 +12337,7 @@
         <v>61</v>
       </c>
       <c r="O12" s="20" t="s">
-        <v>262</v>
+        <v>249</v>
       </c>
       <c r="P12" s="26"/>
     </row>
@@ -12355,7 +12352,7 @@
         <v>84</v>
       </c>
       <c r="D13" s="31" t="s">
-        <v>212</v>
+        <v>276</v>
       </c>
       <c r="E13" s="31" t="s">
         <v>60</v>
@@ -12394,7 +12391,7 @@
     </row>
     <row r="14" spans="1:16" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="33" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="B14" s="34">
         <v>-1</v>
@@ -12404,7 +12401,7 @@
       </c>
       <c r="D14" s="31"/>
       <c r="E14" s="31" t="s">
-        <v>91</v>
+        <v>268</v>
       </c>
       <c r="F14" s="31" t="s">
         <v>61</v>
@@ -12434,7 +12431,7 @@
         <v>61</v>
       </c>
       <c r="O14" s="31" t="s">
-        <v>263</v>
+        <v>250</v>
       </c>
       <c r="P14" s="33"/>
     </row>
@@ -12570,7 +12567,7 @@
         <v>39</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="15"/>
@@ -12588,7 +12585,7 @@
         <v>42</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="15"/>
@@ -12690,7 +12687,7 @@
     </row>
     <row r="12" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="26" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="B12" s="27">
         <v>-1</v>
@@ -12700,7 +12697,7 @@
       </c>
       <c r="D12" s="20"/>
       <c r="E12" s="20" t="s">
-        <v>91</v>
+        <v>268</v>
       </c>
       <c r="F12" s="20" t="s">
         <v>61</v>
@@ -12730,13 +12727,13 @@
         <v>61</v>
       </c>
       <c r="O12" s="20" t="s">
-        <v>263</v>
+        <v>250</v>
       </c>
       <c r="P12" s="26"/>
     </row>
     <row r="13" spans="1:16" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="33" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="B13" s="40">
         <v>0</v>
@@ -12745,7 +12742,7 @@
         <v>48</v>
       </c>
       <c r="D13" s="42" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="E13" s="31" t="s">
         <v>60</v>
@@ -12754,7 +12751,7 @@
         <v>61</v>
       </c>
       <c r="G13" s="31" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H13" s="31" t="s">
         <v>62</v>
@@ -12778,13 +12775,13 @@
         <v>61</v>
       </c>
       <c r="O13" s="31" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="P13" s="33"/>
     </row>
     <row r="14" spans="1:16" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="33" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="B14" s="40">
         <v>-1</v>
@@ -12800,7 +12797,7 @@
         <v>61</v>
       </c>
       <c r="G14" s="31" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H14" s="31" t="s">
         <v>62</v>
@@ -12824,7 +12821,7 @@
         <v>61</v>
       </c>
       <c r="O14" s="31" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="P14" s="33"/>
     </row>

</xml_diff>